<commit_message>
Updated 8.7-8.11 Weekly Report
</commit_message>
<xml_diff>
--- a/Report/周报.xlsx
+++ b/Report/周报.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanwang/Documents/Work/Jiaanpei/Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan\Documents\GitHub\jiaanpei\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>姓名</t>
   </si>
@@ -86,24 +86,29 @@
     <t>8.7-8.11</t>
   </si>
   <si>
-    <t>1. 福耀玻璃数据对接；2. 嘉利供货数据对接与分析；3.学习VIN解析规则，初步做出规划；4.车型定义规则确定</t>
+    <t>1. 基本数据分析；2.供货数据对接和更新（可能有优闪订、车享配、福耀和路鹏等）；3.完成对汽车品牌、车系编码，并细化车型定义和编码规则；4.与明觉、翱特交流数据配件数据结构等</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 后台及本地数据提取和分析；2. 嘉利、优闪订供货数据更新；3.启动和湖北乘用车供应商数据对接（路鹏）；4.参与询价单数据清洗、BI报表制作方案讨论；5.开始筹划建立平台车型库，并进行编码（初步计划对常见115乘用车品牌，14商用车品牌，以及1600余车系和16000余车型进行编码）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -412,13 +417,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -689,20 +697,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="43.83203125" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="43.875" customWidth="1"/>
+    <col min="4" max="4" width="44.375" customWidth="1"/>
+    <col min="5" max="5" width="43.875" customWidth="1"/>
+    <col min="6" max="6" width="27.875" customWidth="1"/>
+    <col min="7" max="7" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -718,7 +726,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -748,7 +756,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">
@@ -774,7 +782,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="323" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="323.10000000000002" customHeight="1">
       <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
@@ -782,7 +790,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>17</v>
@@ -804,7 +812,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18" t="s">
@@ -830,10 +838,12 @@
       <c r="M5" s="7"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="114.75" customHeight="1">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
+      <c r="C6" s="18" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="18" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Update 8.14-8.18 weekly report
</commit_message>
<xml_diff>
--- a/Report/周报.xlsx
+++ b/Report/周报.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan\Documents\GitHub\jiaanpei\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanwang/Documents/Work/Jiaanpei/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,15 +47,6 @@
     <t>数据研发与分析</t>
   </si>
   <si>
-    <t>7.10-7.14</t>
-  </si>
-  <si>
-    <t>1.基本数据分析；2.确立平台数据架构；3.浙江试点相关工作：参与方案编写、流程梳理和app开发、数据接入等</t>
-  </si>
-  <si>
-    <t>1.浙江试点相关工作；2.上货数据架构设计；3.车享配数据分析整理；4.验证明觉数据准确性</t>
-  </si>
-  <si>
     <t>7.17-7.21</t>
   </si>
   <si>
@@ -92,23 +83,32 @@
   <si>
     <t>1. 后台及本地数据提取和分析；2. 嘉利、优闪订供货数据更新；3.启动和湖北乘用车供应商数据对接（路鹏）；4.参与询价单数据清洗、BI报表制作方案讨论；5.开始筹划建立平台车型库，并进行编码（初步计划对常见115乘用车品牌，14商用车品牌，以及1600余车系和16000余车型进行编码）</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.14-8.18</t>
+  </si>
+  <si>
+    <t>1.数据分析；2.数据库状态标识统一化；3.完善定损机构代码和名称对应关系；</t>
+  </si>
+  <si>
+    <t>1.运营数据分析——客服每日周月统计（王文），绵阳每日周月订单及供应商供货情况统计（王国建），每日9、12、15点定时询价单提醒推送（王文），每日询价单及汇总（周彬），出险车主数量更新（王旸）；2.明觉、正时、Audatex+globalInPart数据及业务领域交流</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -135,6 +135,22 @@
       <family val="4"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -347,8 +363,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -416,8 +436,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -697,20 +721,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="43.875" customWidth="1"/>
-    <col min="4" max="4" width="44.375" customWidth="1"/>
-    <col min="5" max="5" width="43.875" customWidth="1"/>
-    <col min="6" max="6" width="27.875" customWidth="1"/>
-    <col min="7" max="7" width="26.875" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="43.83203125" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" customWidth="1"/>
+    <col min="6" max="6" width="43.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -726,7 +750,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -756,7 +780,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">
@@ -782,21 +806,21 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" ht="323.10000000000002" customHeight="1">
+    <row r="4" spans="1:14" ht="323" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="18" t="s">
         <v>10</v>
@@ -812,7 +836,7 @@
       <c r="M4" s="7"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18" t="s">
@@ -838,7 +862,7 @@
       <c r="M5" s="7"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="114.75" customHeight="1">
+    <row r="6" spans="1:14" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18" t="s">
@@ -848,7 +872,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>11</v>

</xml_diff>